<commit_message>
12.17 pre php évfzh
</commit_message>
<xml_diff>
--- a/ÁTLAG.xlsx
+++ b/ÁTLAG.xlsx
@@ -190,7 +190,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -209,6 +209,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="12">
     <border>
@@ -365,7 +371,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1">
       <protection locked="0"/>
@@ -428,6 +434,9 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -738,7 +747,7 @@
   <dimension ref="A1:T23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -811,11 +820,11 @@
         <v>2</v>
       </c>
       <c r="C4" s="10">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D4" s="18">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="T4" s="1" t="s">
         <v>5</v>
@@ -864,12 +873,12 @@
       <c r="B7" s="19">
         <v>5</v>
       </c>
-      <c r="C7" s="10">
-        <v>4</v>
+      <c r="C7" s="21">
+        <v>5</v>
       </c>
       <c r="D7" s="18">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="T7" s="1" t="s">
         <v>8</v>
@@ -882,7 +891,7 @@
       <c r="B8" s="19">
         <v>3</v>
       </c>
-      <c r="C8" s="10">
+      <c r="C8" s="21">
         <v>5</v>
       </c>
       <c r="D8" s="18">
@@ -901,11 +910,11 @@
         <v>3</v>
       </c>
       <c r="C9" s="10">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D9" s="18">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="T9" s="1" t="s">
         <v>10</v>
@@ -955,11 +964,11 @@
         <v>3</v>
       </c>
       <c r="C12" s="10">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D12" s="18">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="T12" s="1" t="s">
         <v>13</v>
@@ -1049,7 +1058,7 @@
       </c>
       <c r="B21" s="5">
         <f>SUMIF(C2:C18,"&gt;"&amp;1,D2:D18)/SUMIF(C2:C18,"&gt;"&amp;1,B2:B18)</f>
-        <v>4.1111111111111107</v>
+        <v>4.0555555555555554</v>
       </c>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.25">
@@ -1058,7 +1067,7 @@
       </c>
       <c r="B22" s="6">
         <f>SUMIF(C2:C18,"&gt;"&amp;1,D2:D18)/30</f>
-        <v>4.9333333333333336</v>
+        <v>4.8666666666666663</v>
       </c>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.25">

</xml_diff>